<commit_message>
Support for all valves
Five different outputs have been added to the PLC program.  The timing
still needs some work before it is ready.
</commit_message>
<xml_diff>
--- a/Valve State Table.xlsx
+++ b/Valve State Table.xlsx
@@ -46,7 +46,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -54,16 +54,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -71,16 +89,43 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -384,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -419,92 +464,332 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1" t="s">
+      <c r="C7" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="G7" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="1">
-        <v>1</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1">
+      <c r="C8" s="3">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4">
+        <v>1</v>
+      </c>
+      <c r="E8" s="5">
+        <v>0</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
+        <v>0</v>
+      </c>
+      <c r="H8" s="5">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="1">
+      <c r="C9" s="3">
         <v>2</v>
       </c>
+      <c r="D9" s="4">
+        <v>1</v>
+      </c>
+      <c r="E9" s="5">
+        <v>0</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <v>0</v>
+      </c>
+      <c r="H9" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="1">
+      <c r="C10" s="3">
         <v>3</v>
       </c>
+      <c r="D10" s="5">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4">
+        <v>1</v>
+      </c>
+      <c r="F10" s="5">
+        <v>0</v>
+      </c>
+      <c r="G10" s="5">
+        <v>0</v>
+      </c>
+      <c r="H10" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="1">
+      <c r="C11" s="3">
         <v>4</v>
       </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4">
+        <v>1</v>
+      </c>
+      <c r="F11" s="5">
+        <v>0</v>
+      </c>
+      <c r="G11" s="5">
+        <v>0</v>
+      </c>
+      <c r="H11" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="1">
+      <c r="C12" s="3">
         <v>5</v>
       </c>
+      <c r="D12" s="5">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5">
+        <v>0</v>
+      </c>
+      <c r="F12" s="4">
+        <v>1</v>
+      </c>
+      <c r="G12" s="5">
+        <v>0</v>
+      </c>
+      <c r="H12" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C13" s="1">
+      <c r="C13" s="3">
         <v>6</v>
       </c>
+      <c r="D13" s="5">
+        <v>0</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
+      <c r="F13" s="4">
+        <v>1</v>
+      </c>
+      <c r="G13" s="5">
+        <v>0</v>
+      </c>
+      <c r="H13" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C14" s="1">
+      <c r="C14" s="3">
         <v>7</v>
       </c>
+      <c r="D14" s="5">
+        <v>0</v>
+      </c>
+      <c r="E14" s="5">
+        <v>0</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0</v>
+      </c>
+      <c r="G14" s="4">
+        <v>1</v>
+      </c>
+      <c r="H14" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="1">
+      <c r="C15" s="3">
         <v>8</v>
       </c>
+      <c r="D15" s="5">
+        <v>0</v>
+      </c>
+      <c r="E15" s="5">
+        <v>0</v>
+      </c>
+      <c r="F15" s="5">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4">
+        <v>1</v>
+      </c>
+      <c r="H15" s="5">
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="1">
+      <c r="C16" s="3">
         <v>9</v>
       </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" s="1">
+      <c r="D16" s="5">
+        <v>0</v>
+      </c>
+      <c r="E16" s="5">
+        <v>0</v>
+      </c>
+      <c r="F16" s="5">
+        <v>0</v>
+      </c>
+      <c r="G16" s="5">
+        <v>0</v>
+      </c>
+      <c r="H16" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C17" s="3">
         <v>10</v>
       </c>
+      <c r="D17" s="5">
+        <v>0</v>
+      </c>
+      <c r="E17" s="5">
+        <v>0</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0</v>
+      </c>
+      <c r="G17" s="5">
+        <v>0</v>
+      </c>
+      <c r="H17" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+    </row>
+    <row r="21" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="3"/>
+    </row>
+    <row r="23" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+    </row>
+    <row r="25" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+    </row>
+    <row r="26" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="3"/>
+    </row>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+    </row>
+    <row r="28" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+    </row>
+    <row r="29" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+    </row>
+    <row r="30" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>